<commit_message>
done with login and logout functionality
</commit_message>
<xml_diff>
--- a/Team7_Dollardays/testdata/testdata.xlsx
+++ b/Team7_Dollardays/testdata/testdata.xlsx
@@ -8,21 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shachi\GitStuff\Dollardays\Team7_Dollardays\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9208362E-3BAA-409C-B172-A93A0393EAFE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B6A3A48-1CB0-4BCE-B1DD-955213A4717F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Login&amp;Logout" sheetId="1" r:id="rId1"/>
-    <sheet name="SubmitRequest" sheetId="2" r:id="rId2"/>
-    <sheet name="Menu" sheetId="3" r:id="rId3"/>
+    <sheet name="Login" sheetId="1" r:id="rId1"/>
+    <sheet name="Logout" sheetId="4" r:id="rId2"/>
+    <sheet name="SubmitRequest" sheetId="2" r:id="rId3"/>
+    <sheet name="Menu" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="63">
   <si>
     <t>TCID</t>
   </si>
@@ -205,6 +206,12 @@
   </si>
   <si>
     <t>Submit A Request</t>
+  </si>
+  <si>
+    <t>Logout from user toggle button</t>
+  </si>
+  <si>
+    <t>Logout from User Account Page</t>
   </si>
 </sst>
 </file>
@@ -632,8 +639,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -687,6 +694,81 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38EF0EC1-3A1B-4CD6-940E-FDAE6F9681BB}">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="34.5546875" customWidth="1"/>
+    <col min="4" max="4" width="26.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{BF7E7821-8270-4CA5-80DB-1720A407DF85}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{567BFC49-CCFB-4294-A574-A2D3A42E43F2}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Q15"/>
   <sheetViews>
@@ -1154,7 +1236,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
Logout Test case update
</commit_message>
<xml_diff>
--- a/Team7_Dollardays/testdata/testdata.xlsx
+++ b/Team7_Dollardays/testdata/testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shachi\GitStuff\Dollardays\Team7_Dollardays\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B6A3A48-1CB0-4BCE-B1DD-955213A4717F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6477B92-45CF-429C-8C51-9E145104B167}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="66">
   <si>
     <t>TCID</t>
   </si>
@@ -212,6 +212,15 @@
   </si>
   <si>
     <t>Logout from User Account Page</t>
+  </si>
+  <si>
+    <t>ExptectedResult</t>
+  </si>
+  <si>
+    <t>Logged out from user toggle button.</t>
+  </si>
+  <si>
+    <t>Logged out from Account web page.</t>
   </si>
 </sst>
 </file>
@@ -695,10 +704,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38EF0EC1-3A1B-4CD6-940E-FDAE6F9681BB}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -706,9 +715,10 @@
     <col min="2" max="2" width="34.5546875" customWidth="1"/>
     <col min="4" max="4" width="26.5546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -724,8 +734,11 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -741,8 +754,11 @@
       <c r="E2" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -757,6 +773,9 @@
       </c>
       <c r="E3" s="2" t="s">
         <v>8</v>
+      </c>
+      <c r="F3" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>